<commit_message>
Delete course equivalencies when program deleted
</commit_message>
<xml_diff>
--- a/spreadsheets/sponsored_2019.xlsx
+++ b/spreadsheets/sponsored_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Norman\Desktop\zags-abroad\zags-abroad-backend\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krist\OneDrive - Gonzaga University\Senior Design\zags-abroad-backend\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BBDA5A-88E5-43EA-8BFA-0A0AEA0133E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00E2B27-7015-44A9-8D5B-2CDD80FDDC32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL EQUIVALENCIES use Filter " sheetId="1" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10542" uniqueCount="3548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10610" uniqueCount="3583">
   <si>
     <t>Program/Host</t>
   </si>
@@ -10704,6 +10703,111 @@
   </si>
   <si>
     <t>Queensland, Australia</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10003</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10236</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10043</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10317</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10060</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10196</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10138</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10012</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10107</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10025</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10030</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10200</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10199</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10151</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10052</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10005</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10022</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10057</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10050</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10144</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10125</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10179</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10152</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10034</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10037</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10143</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10035</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10036</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10039</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10001</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10046</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10116</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10308</t>
+  </si>
+  <si>
+    <t>https://studyabroad.gonzaga.edu/index.cfm?FuseAction=Programs.ViewProgram&amp;Program_ID=10068</t>
   </si>
 </sst>
 </file>
@@ -10883,7 +10987,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10966,6 +11070,15 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11346,8 +11459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A345" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A364" sqref="A364"/>
+    <sheetView topLeftCell="A345" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C359" sqref="C359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -53233,7 +53346,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:A1269" xr:uid="{3B9032D9-4CE6-4543-8D9D-8F842B5BC94E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L1269">
+  <sortState ref="A2:L1269">
     <sortCondition ref="A118"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -53246,21 +53359,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D59CD3-977B-4D90-81C0-6F8F1973F74E}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.15"/>
+  <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
-    <col min="1" max="1" width="25.8125" style="51" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5625" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.8125" style="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3125" style="51" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.9375" style="51" customWidth="1"/>
+    <col min="2" max="2" width="7.0625" style="51" customWidth="1"/>
+    <col min="3" max="3" width="6.3125" style="51" customWidth="1"/>
+    <col min="4" max="4" width="56.4375" style="56" customWidth="1"/>
     <col min="5" max="5" width="23.25" style="51" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="10.5">
+    <row r="1" spans="1:7">
       <c r="A1" s="50" t="s">
         <v>3289</v>
       </c>
@@ -53270,7 +53383,7 @@
       <c r="C1" s="50" t="s">
         <v>3291</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="54" t="s">
         <v>3292</v>
       </c>
       <c r="E1" s="50" t="s">
@@ -53283,13 +53396,17 @@
         <v>3295</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="10.5">
+    <row r="2" spans="1:7">
       <c r="A2" s="52" t="s">
         <v>2742</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
+      <c r="D2" s="54" t="s">
+        <v>3548</v>
+      </c>
       <c r="E2" s="50" t="s">
         <v>3296</v>
       </c>
@@ -53300,13 +53417,17 @@
         <v>-0.12775829999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="10.5">
+    <row r="3" spans="1:7">
       <c r="A3" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="50"/>
+      <c r="B3" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="D3" s="54" t="s">
+        <v>3549</v>
+      </c>
       <c r="E3" s="50" t="s">
         <v>3297</v>
       </c>
@@ -53317,13 +53438,17 @@
         <v>2.3522219</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="10.5">
+    <row r="4" spans="1:7">
       <c r="A4" s="52" t="s">
         <v>2817</v>
       </c>
-      <c r="B4" s="50"/>
+      <c r="B4" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
+      <c r="D4" s="54" t="s">
+        <v>3578</v>
+      </c>
       <c r="E4" s="50" t="s">
         <v>3298</v>
       </c>
@@ -53334,13 +53459,17 @@
         <v>18.860151999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="10.5">
+    <row r="5" spans="1:7">
       <c r="A5" s="52" t="s">
         <v>232</v>
       </c>
-      <c r="B5" s="50"/>
+      <c r="B5" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
+      <c r="D5" s="54" t="s">
+        <v>3550</v>
+      </c>
       <c r="E5" s="50" t="s">
         <v>3299</v>
       </c>
@@ -53351,13 +53480,17 @@
         <v>140.1023643</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="10.5">
+    <row r="6" spans="1:7">
       <c r="A6" s="52" t="s">
         <v>2852</v>
       </c>
-      <c r="B6" s="50"/>
+      <c r="B6" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
+      <c r="D6" s="54" t="s">
+        <v>3551</v>
+      </c>
       <c r="E6" s="53" t="s">
         <v>3547</v>
       </c>
@@ -53368,13 +53501,17 @@
         <v>153.4166377</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="10.5">
+    <row r="7" spans="1:7">
       <c r="A7" s="52" t="s">
         <v>370</v>
       </c>
-      <c r="B7" s="50"/>
+      <c r="B7" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
+      <c r="D7" s="54" t="s">
+        <v>3552</v>
+      </c>
       <c r="E7" s="50" t="s">
         <v>3300</v>
       </c>
@@ -53385,13 +53522,17 @@
         <v>-64.188776099999998</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="10.5">
+    <row r="8" spans="1:7">
       <c r="A8" s="53" t="s">
         <v>377</v>
       </c>
-      <c r="B8" s="50"/>
+      <c r="B8" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
+      <c r="D8" s="54" t="s">
+        <v>3554</v>
+      </c>
       <c r="E8" s="50" t="s">
         <v>3301</v>
       </c>
@@ -53402,13 +53543,17 @@
         <v>35.928371599999998</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="10.5">
+    <row r="9" spans="1:7">
       <c r="A9" s="53" t="s">
         <v>442</v>
       </c>
-      <c r="B9" s="50"/>
+      <c r="B9" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
+      <c r="D9" s="54" t="s">
+        <v>3555</v>
+      </c>
       <c r="E9" s="50" t="s">
         <v>3302</v>
       </c>
@@ -53419,13 +53564,17 @@
         <v>78.486671000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="10.5">
+    <row r="10" spans="1:7">
       <c r="A10" s="52" t="s">
         <v>2816</v>
       </c>
-      <c r="B10" s="50"/>
+      <c r="B10" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
+      <c r="D10" s="54" t="s">
+        <v>3556</v>
+      </c>
       <c r="E10" s="50" t="s">
         <v>3303</v>
       </c>
@@ -53436,13 +53585,17 @@
         <v>12.5683372</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="10.5">
+    <row r="11" spans="1:7">
       <c r="A11" s="52" t="s">
         <v>583</v>
       </c>
-      <c r="B11" s="50"/>
+      <c r="B11" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
+      <c r="D11" s="54" t="s">
+        <v>3557</v>
+      </c>
       <c r="E11" s="50" t="s">
         <v>3304</v>
       </c>
@@ -53453,13 +53606,17 @@
         <v>5.4474269999999896</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="10.5">
+    <row r="12" spans="1:7">
       <c r="A12" s="52" t="s">
         <v>744</v>
       </c>
-      <c r="B12" s="50"/>
+      <c r="B12" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
+      <c r="D12" s="54" t="s">
+        <v>3558</v>
+      </c>
       <c r="E12" s="50" t="s">
         <v>3305</v>
       </c>
@@ -53470,13 +53627,17 @@
         <v>-58.381559099999997</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="10.5">
+    <row r="13" spans="1:7">
       <c r="A13" s="52" t="s">
         <v>762</v>
       </c>
-      <c r="B13" s="50"/>
+      <c r="B13" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
+      <c r="D13" s="54" t="s">
+        <v>3559</v>
+      </c>
       <c r="E13" s="53" t="s">
         <v>3306</v>
       </c>
@@ -53487,13 +53648,17 @@
         <v>-71.612688499999905</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="10.5">
+    <row r="14" spans="1:7">
       <c r="A14" s="52" t="s">
         <v>857</v>
       </c>
-      <c r="B14" s="50"/>
+      <c r="B14" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
+      <c r="D14" s="54" t="s">
+        <v>3560</v>
+      </c>
       <c r="E14" s="53" t="s">
         <v>3309</v>
       </c>
@@ -53504,13 +53669,17 @@
         <v>15.439503999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="10.5">
+    <row r="15" spans="1:7">
       <c r="A15" s="52" t="s">
         <v>3307</v>
       </c>
-      <c r="B15" s="50"/>
+      <c r="B15" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
+      <c r="D15" s="54" t="s">
+        <v>3561</v>
+      </c>
       <c r="E15" s="53" t="s">
         <v>3308</v>
       </c>
@@ -53521,13 +53690,17 @@
         <v>4.3517210999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="10.5">
+    <row r="16" spans="1:7">
       <c r="A16" s="52" t="s">
         <v>897</v>
       </c>
-      <c r="B16" s="50"/>
+      <c r="B16" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
+      <c r="D16" s="54" t="s">
+        <v>3562</v>
+      </c>
       <c r="E16" s="53" t="s">
         <v>3310</v>
       </c>
@@ -53538,13 +53711,17 @@
         <v>-0.16135920000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="10.5">
+    <row r="17" spans="1:7">
       <c r="A17" s="53" t="s">
         <v>991</v>
       </c>
-      <c r="B17" s="50"/>
+      <c r="B17" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
+      <c r="D17" s="54" t="s">
+        <v>3582</v>
+      </c>
       <c r="E17" s="53" t="s">
         <v>3311</v>
       </c>
@@ -53555,13 +53732,17 @@
         <v>12.4963655</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="10.5">
+    <row r="18" spans="1:7">
       <c r="A18" s="52" t="s">
         <v>1017</v>
       </c>
-      <c r="B18" s="50"/>
+      <c r="B18" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
+      <c r="D18" s="54" t="s">
+        <v>3563</v>
+      </c>
       <c r="E18" s="53" t="s">
         <v>3312</v>
       </c>
@@ -53572,13 +53753,17 @@
         <v>-1.2577263000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="10.5">
+    <row r="19" spans="1:7">
       <c r="A19" s="52" t="s">
         <v>3018</v>
       </c>
-      <c r="B19" s="50"/>
+      <c r="B19" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
+      <c r="D19" s="54" t="s">
+        <v>3564</v>
+      </c>
       <c r="E19" s="53" t="s">
         <v>3296</v>
       </c>
@@ -53589,13 +53774,17 @@
         <v>-0.12775829999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="10.5">
+    <row r="20" spans="1:7">
       <c r="A20" s="53" t="s">
         <v>1316</v>
       </c>
-      <c r="B20" s="50"/>
+      <c r="B20" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
+      <c r="D20" s="55" t="s">
+        <v>3573</v>
+      </c>
       <c r="E20" s="53" t="s">
         <v>3313</v>
       </c>
@@ -53606,13 +53795,17 @@
         <v>145.48585990000001</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="10.5">
+    <row r="21" spans="1:7">
       <c r="A21" s="53" t="s">
         <v>1335</v>
       </c>
-      <c r="B21" s="50"/>
+      <c r="B21" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
+      <c r="D21" s="55" t="s">
+        <v>3571</v>
+      </c>
       <c r="E21" s="53" t="s">
         <v>3314</v>
       </c>
@@ -53623,13 +53816,17 @@
         <v>90.677304599999999</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="10.5">
+    <row r="22" spans="1:7">
       <c r="A22" s="53" t="s">
         <v>1348</v>
       </c>
-      <c r="B22" s="50"/>
+      <c r="B22" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
+      <c r="D22" s="55" t="s">
+        <v>3574</v>
+      </c>
       <c r="E22" s="53" t="s">
         <v>3315</v>
       </c>
@@ -53640,13 +53837,17 @@
         <v>103.85517299999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="10.5">
+    <row r="23" spans="1:7">
       <c r="A23" s="53" t="s">
         <v>1359</v>
       </c>
-      <c r="B23" s="50"/>
+      <c r="B23" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
+      <c r="D23" s="55" t="s">
+        <v>3575</v>
+      </c>
       <c r="E23" s="53" t="s">
         <v>3316</v>
       </c>
@@ -53657,13 +53858,17 @@
         <v>-84.373839399999994</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="10.5">
+    <row r="24" spans="1:7">
       <c r="A24" s="53" t="s">
         <v>1368</v>
       </c>
-      <c r="B24" s="50"/>
+      <c r="B24" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
+      <c r="D24" s="55" t="s">
+        <v>3576</v>
+      </c>
       <c r="E24" s="53" t="s">
         <v>3317</v>
       </c>
@@ -53674,13 +53879,17 @@
         <v>-82.520778699999994</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="10.5">
+    <row r="25" spans="1:7">
       <c r="A25" s="53" t="s">
         <v>1374</v>
       </c>
-      <c r="B25" s="50"/>
+      <c r="B25" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
+      <c r="D25" s="55" t="s">
+        <v>3570</v>
+      </c>
       <c r="E25" s="53" t="s">
         <v>3318</v>
       </c>
@@ -53691,13 +53900,17 @@
         <v>-71.967462599999905</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="10.5">
+    <row r="26" spans="1:7">
       <c r="A26" s="52" t="s">
         <v>1382</v>
       </c>
-      <c r="B26" s="50"/>
+      <c r="B26" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
+      <c r="D26" s="55" t="s">
+        <v>3577</v>
+      </c>
       <c r="E26" s="53" t="s">
         <v>3319</v>
       </c>
@@ -53708,13 +53921,17 @@
         <v>35.734195300000003</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="10.5">
+    <row r="27" spans="1:7">
       <c r="A27" s="53" t="s">
         <v>1394</v>
       </c>
-      <c r="B27" s="50"/>
+      <c r="B27" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
+      <c r="D27" s="55" t="s">
+        <v>3572</v>
+      </c>
       <c r="E27" s="53" t="s">
         <v>3320</v>
       </c>
@@ -53725,13 +53942,17 @@
         <v>-71.518979999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="10.5">
+    <row r="28" spans="1:7">
       <c r="A28" s="52" t="s">
         <v>1399</v>
       </c>
-      <c r="B28" s="50"/>
+      <c r="B28" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
+      <c r="D28" s="54" t="s">
+        <v>3579</v>
+      </c>
       <c r="E28" s="53" t="s">
         <v>3321</v>
       </c>
@@ -53742,13 +53963,17 @@
         <v>139.69170639999999</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="10.5">
+    <row r="29" spans="1:7">
       <c r="A29" s="52" t="s">
         <v>2818</v>
       </c>
-      <c r="B29" s="50"/>
+      <c r="B29" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
+      <c r="D29" s="54" t="s">
+        <v>3580</v>
+      </c>
       <c r="E29" s="53" t="s">
         <v>3322</v>
       </c>
@@ -53759,13 +53984,17 @@
         <v>-3.7037901999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="10.5">
+    <row r="30" spans="1:7">
       <c r="A30" s="52" t="s">
         <v>1795</v>
       </c>
-      <c r="B30" s="50"/>
+      <c r="B30" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
+      <c r="D30" s="54" t="s">
+        <v>3581</v>
+      </c>
       <c r="E30" s="53" t="s">
         <v>3323</v>
       </c>
@@ -53776,13 +54005,17 @@
         <v>116.4073963</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="10.5">
+    <row r="31" spans="1:7">
       <c r="A31" s="52" t="s">
         <v>1841</v>
       </c>
-      <c r="B31" s="50"/>
+      <c r="B31" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
+      <c r="D31" s="54" t="s">
+        <v>3565</v>
+      </c>
       <c r="E31" s="53" t="s">
         <v>3324</v>
       </c>
@@ -53793,13 +54026,17 @@
         <v>174.76333149999999</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="10.5">
+    <row r="32" spans="1:7">
       <c r="A32" s="52" t="s">
         <v>2171</v>
       </c>
-      <c r="B32" s="50"/>
+      <c r="B32" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
+      <c r="D32" s="54" t="s">
+        <v>3566</v>
+      </c>
       <c r="E32" s="53" t="s">
         <v>3325</v>
       </c>
@@ -53810,13 +54047,17 @@
         <v>-4.2518060000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="10.5">
+    <row r="33" spans="1:7">
       <c r="A33" s="52" t="s">
         <v>2559</v>
       </c>
-      <c r="B33" s="50"/>
+      <c r="B33" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
+      <c r="D33" s="54" t="s">
+        <v>3567</v>
+      </c>
       <c r="E33" s="53" t="s">
         <v>3326</v>
       </c>
@@ -53827,13 +54068,17 @@
         <v>-3.5985570999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="10.5">
+    <row r="34" spans="1:7">
       <c r="A34" s="52" t="s">
         <v>2627</v>
       </c>
-      <c r="B34" s="50"/>
+      <c r="B34" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
+      <c r="D34" s="54" t="s">
+        <v>3568</v>
+      </c>
       <c r="E34" s="53" t="s">
         <v>3327</v>
       </c>
@@ -53844,13 +54089,17 @@
         <v>-8.6267343000000007</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="10.5">
+    <row r="35" spans="1:7">
       <c r="A35" s="53" t="s">
         <v>2690</v>
       </c>
-      <c r="B35" s="50"/>
+      <c r="B35" s="50" t="s">
+        <v>3553</v>
+      </c>
       <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
+      <c r="D35" s="54" t="s">
+        <v>3569</v>
+      </c>
       <c r="E35" s="53" t="s">
         <v>3328</v>
       </c>
@@ -53863,7 +54112,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:A36" xr:uid="{E0F9AFD1-752F-46CC-9D8C-A798927D6393}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G35">
+  <sortState ref="A2:G35">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update program script and db
</commit_message>
<xml_diff>
--- a/spreadsheets/sponsored_2019.xlsx
+++ b/spreadsheets/sponsored_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krist\OneDrive - Gonzaga University\Senior Design\zags-abroad-backend\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00E2B27-7015-44A9-8D5B-2CDD80FDDC32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893ACFAB-7402-4674-9BA5-0E5C8AEF847E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10610" uniqueCount="3583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10609" uniqueCount="3582">
   <si>
     <t>Program/Host</t>
   </si>
@@ -9932,9 +9932,6 @@
   </si>
   <si>
     <t>PROGRAM TYPE</t>
-  </si>
-  <si>
-    <t>HOST URL</t>
   </si>
   <si>
     <t>APPLICATION LINK</t>
@@ -23400,7 +23397,7 @@
     </row>
     <row r="363" spans="1:12" ht="13.9">
       <c r="A363" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B363" s="3" t="s">
         <v>947</v>
@@ -23437,7 +23434,7 @@
     </row>
     <row r="364" spans="1:12" ht="13.9">
       <c r="A364" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B364" s="3" t="s">
         <v>949</v>
@@ -23469,7 +23466,7 @@
     </row>
     <row r="365" spans="1:12" ht="13.9">
       <c r="A365" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B365" s="3" t="s">
         <v>3009</v>
@@ -23501,7 +23498,7 @@
     </row>
     <row r="366" spans="1:12" ht="13.9">
       <c r="A366" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B366" s="3" t="s">
         <v>954</v>
@@ -23533,7 +23530,7 @@
     </row>
     <row r="367" spans="1:12" ht="13.9">
       <c r="A367" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B367" s="3" t="s">
         <v>958</v>
@@ -23567,7 +23564,7 @@
     </row>
     <row r="368" spans="1:12" ht="13.9">
       <c r="A368" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B368" s="3" t="s">
         <v>960</v>
@@ -23599,7 +23596,7 @@
     </row>
     <row r="369" spans="1:13" ht="13.9">
       <c r="A369" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B369" s="3" t="s">
         <v>962</v>
@@ -23631,7 +23628,7 @@
     </row>
     <row r="370" spans="1:13" ht="13.9">
       <c r="A370" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B370" s="3" t="s">
         <v>3010</v>
@@ -23663,7 +23660,7 @@
     </row>
     <row r="371" spans="1:13" ht="13.9">
       <c r="A371" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B371" s="3" t="s">
         <v>966</v>
@@ -23697,7 +23694,7 @@
     </row>
     <row r="372" spans="1:13" ht="13.9">
       <c r="A372" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B372" s="3" t="s">
         <v>968</v>
@@ -23731,7 +23728,7 @@
     </row>
     <row r="373" spans="1:13" ht="13.9">
       <c r="A373" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B373" s="3" t="s">
         <v>3007</v>
@@ -23763,7 +23760,7 @@
     </row>
     <row r="374" spans="1:13" ht="13.9">
       <c r="A374" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B374" s="3" t="s">
         <v>2765</v>
@@ -23797,7 +23794,7 @@
     </row>
     <row r="375" spans="1:13" ht="13.9">
       <c r="A375" s="3" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="B375" s="3" t="s">
         <v>3008</v>
@@ -53357,33 +53354,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D59CD3-977B-4D90-81C0-6F8F1973F74E}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
     <col min="1" max="1" width="17.9375" style="51" customWidth="1"/>
     <col min="2" max="2" width="7.0625" style="51" customWidth="1"/>
-    <col min="3" max="3" width="6.3125" style="51" customWidth="1"/>
-    <col min="4" max="4" width="56.4375" style="56" customWidth="1"/>
-    <col min="5" max="5" width="23.25" style="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="51"/>
+    <col min="3" max="3" width="56.4375" style="56" customWidth="1"/>
+    <col min="4" max="4" width="23.25" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="50" t="s">
         <v>3289</v>
       </c>
       <c r="B1" s="50" t="s">
         <v>3290</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="54" t="s">
         <v>3291</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="50" t="s">
         <v>3292</v>
       </c>
       <c r="E1" s="50" t="s">
@@ -53392,727 +53388,690 @@
       <c r="F1" s="50" t="s">
         <v>3294</v>
       </c>
-      <c r="G1" s="50" t="s">
-        <v>3295</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="52" t="s">
         <v>2742</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="54" t="s">
-        <v>3548</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>3296</v>
+        <v>3552</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>3547</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>3295</v>
+      </c>
+      <c r="E2" s="50">
+        <v>51.507350899999999</v>
       </c>
       <c r="F2" s="50">
-        <v>51.507350899999999</v>
-      </c>
-      <c r="G2" s="50">
         <v>-0.12775829999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" s="52" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="54" t="s">
-        <v>3549</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>3297</v>
+        <v>3552</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>3548</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>3296</v>
+      </c>
+      <c r="E3" s="50">
+        <v>48.856614</v>
       </c>
       <c r="F3" s="50">
-        <v>48.856614</v>
-      </c>
-      <c r="G3" s="50">
         <v>2.3522219</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" s="52" t="s">
         <v>2817</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="54" t="s">
-        <v>3578</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>3298</v>
+        <v>3552</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>3577</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>3297</v>
+      </c>
+      <c r="E4" s="50">
+        <v>-33.932104500000001</v>
       </c>
       <c r="F4" s="50">
-        <v>-33.932104500000001</v>
-      </c>
-      <c r="G4" s="50">
         <v>18.860151999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5" s="52" t="s">
         <v>232</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="54" t="s">
-        <v>3550</v>
-      </c>
-      <c r="E5" s="50" t="s">
-        <v>3299</v>
+        <v>3552</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>3549</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>3298</v>
+      </c>
+      <c r="E5" s="50">
+        <v>39.718613499999996</v>
       </c>
       <c r="F5" s="50">
-        <v>39.718613499999996</v>
-      </c>
-      <c r="G5" s="50">
         <v>140.1023643</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6">
       <c r="A6" s="52" t="s">
         <v>2852</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="54" t="s">
-        <v>3551</v>
-      </c>
-      <c r="E6" s="53" t="s">
-        <v>3547</v>
+        <v>3552</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>3550</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>3546</v>
+      </c>
+      <c r="E6" s="50">
+        <v>-28.073093400000001</v>
       </c>
       <c r="F6" s="50">
-        <v>-28.073093400000001</v>
-      </c>
-      <c r="G6" s="50">
         <v>153.4166377</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7" s="52" t="s">
         <v>370</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="54" t="s">
         <v>3552</v>
       </c>
-      <c r="E7" s="50" t="s">
-        <v>3300</v>
+      <c r="C7" s="54" t="s">
+        <v>3551</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>3299</v>
+      </c>
+      <c r="E7" s="50">
+        <v>-31.420083299999899</v>
       </c>
       <c r="F7" s="50">
-        <v>-31.420083299999899</v>
-      </c>
-      <c r="G7" s="50">
         <v>-64.188776099999998</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6">
       <c r="A8" s="53" t="s">
         <v>377</v>
       </c>
       <c r="B8" s="50" t="s">
+        <v>3552</v>
+      </c>
+      <c r="C8" s="54" t="s">
         <v>3553</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="54" t="s">
-        <v>3554</v>
-      </c>
-      <c r="E8" s="50" t="s">
-        <v>3301</v>
+      <c r="D8" s="50" t="s">
+        <v>3300</v>
+      </c>
+      <c r="E8" s="50">
+        <v>31.9453666</v>
       </c>
       <c r="F8" s="50">
-        <v>31.9453666</v>
-      </c>
-      <c r="G8" s="50">
         <v>35.928371599999998</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6">
       <c r="A9" s="53" t="s">
         <v>442</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="54" t="s">
-        <v>3555</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>3302</v>
+        <v>3552</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>3554</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>3301</v>
+      </c>
+      <c r="E9" s="50">
+        <v>17.385044000000001</v>
       </c>
       <c r="F9" s="50">
-        <v>17.385044000000001</v>
-      </c>
-      <c r="G9" s="50">
         <v>78.486671000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6">
       <c r="A10" s="52" t="s">
         <v>2816</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="54" t="s">
-        <v>3556</v>
-      </c>
-      <c r="E10" s="50" t="s">
-        <v>3303</v>
+        <v>3552</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>3555</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>3302</v>
+      </c>
+      <c r="E10" s="50">
+        <v>55.676096800000003</v>
       </c>
       <c r="F10" s="50">
-        <v>55.676096800000003</v>
-      </c>
-      <c r="G10" s="50">
         <v>12.5683372</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6">
       <c r="A11" s="52" t="s">
         <v>583</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="54" t="s">
-        <v>3557</v>
-      </c>
-      <c r="E11" s="50" t="s">
-        <v>3304</v>
+        <v>3552</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>3556</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>3303</v>
+      </c>
+      <c r="E11" s="50">
+        <v>43.529741999999999</v>
       </c>
       <c r="F11" s="50">
-        <v>43.529741999999999</v>
-      </c>
-      <c r="G11" s="50">
         <v>5.4474269999999896</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:6">
       <c r="A12" s="52" t="s">
         <v>744</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="54" t="s">
-        <v>3558</v>
-      </c>
-      <c r="E12" s="50" t="s">
-        <v>3305</v>
+        <v>3552</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>3557</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>3304</v>
+      </c>
+      <c r="E12" s="50">
+        <v>-34.603684399999999</v>
       </c>
       <c r="F12" s="50">
-        <v>-34.603684399999999</v>
-      </c>
-      <c r="G12" s="50">
         <v>-58.381559099999997</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:6">
       <c r="A13" s="52" t="s">
         <v>762</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="54" t="s">
-        <v>3559</v>
-      </c>
-      <c r="E13" s="53" t="s">
-        <v>3306</v>
+        <v>3552</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>3558</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>3305</v>
+      </c>
+      <c r="E13" s="50">
+        <v>-33.047238</v>
       </c>
       <c r="F13" s="50">
-        <v>-33.047238</v>
-      </c>
-      <c r="G13" s="50">
         <v>-71.612688499999905</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:6">
       <c r="A14" s="52" t="s">
         <v>857</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="54" t="s">
+        <v>3552</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>3559</v>
+      </c>
+      <c r="D14" s="53" t="s">
+        <v>3308</v>
+      </c>
+      <c r="E14" s="50">
+        <v>47.070714000000002</v>
+      </c>
+      <c r="F14" s="50">
+        <v>15.439503999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="52" t="s">
+        <v>3306</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>3552</v>
+      </c>
+      <c r="C15" s="54" t="s">
         <v>3560</v>
       </c>
-      <c r="E14" s="53" t="s">
-        <v>3309</v>
-      </c>
-      <c r="F14" s="50">
-        <v>47.070714000000002</v>
-      </c>
-      <c r="G14" s="50">
-        <v>15.439503999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="52" t="s">
+      <c r="D15" s="53" t="s">
         <v>3307</v>
       </c>
-      <c r="B15" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="54" t="s">
-        <v>3561</v>
-      </c>
-      <c r="E15" s="53" t="s">
-        <v>3308</v>
+      <c r="E15" s="50">
+        <v>50.850346299999998</v>
       </c>
       <c r="F15" s="50">
-        <v>50.850346299999998</v>
-      </c>
-      <c r="G15" s="50">
         <v>4.3517210999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:6">
       <c r="A16" s="52" t="s">
         <v>897</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="54" t="s">
-        <v>3562</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>3310</v>
+        <v>3552</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>3561</v>
+      </c>
+      <c r="D16" s="53" t="s">
+        <v>3309</v>
+      </c>
+      <c r="E16" s="50">
+        <v>5.6358281000000003</v>
       </c>
       <c r="F16" s="50">
-        <v>5.6358281000000003</v>
-      </c>
-      <c r="G16" s="50">
         <v>-0.16135920000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:6">
       <c r="A17" s="53" t="s">
         <v>991</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="54" t="s">
-        <v>3582</v>
-      </c>
-      <c r="E17" s="53" t="s">
-        <v>3311</v>
+        <v>3552</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>3581</v>
+      </c>
+      <c r="D17" s="53" t="s">
+        <v>3310</v>
+      </c>
+      <c r="E17" s="50">
+        <v>41.902783499999998</v>
       </c>
       <c r="F17" s="50">
-        <v>41.902783499999998</v>
-      </c>
-      <c r="G17" s="50">
         <v>12.4963655</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:6">
       <c r="A18" s="52" t="s">
         <v>1017</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="54" t="s">
-        <v>3563</v>
-      </c>
-      <c r="E18" s="53" t="s">
-        <v>3312</v>
+        <v>3552</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>3562</v>
+      </c>
+      <c r="D18" s="53" t="s">
+        <v>3311</v>
+      </c>
+      <c r="E18" s="50">
+        <v>51.752020899999998</v>
       </c>
       <c r="F18" s="50">
-        <v>51.752020899999998</v>
-      </c>
-      <c r="G18" s="50">
         <v>-1.2577263000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:6">
       <c r="A19" s="52" t="s">
         <v>3018</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="54" t="s">
-        <v>3564</v>
-      </c>
-      <c r="E19" s="53" t="s">
-        <v>3296</v>
+        <v>3552</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>3563</v>
+      </c>
+      <c r="D19" s="53" t="s">
+        <v>3295</v>
+      </c>
+      <c r="E19" s="50">
+        <v>51.507350899999999</v>
       </c>
       <c r="F19" s="50">
-        <v>51.507350899999999</v>
-      </c>
-      <c r="G19" s="50">
         <v>-0.12775829999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:6">
       <c r="A20" s="53" t="s">
         <v>1316</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="55" t="s">
-        <v>3573</v>
-      </c>
-      <c r="E20" s="53" t="s">
-        <v>3313</v>
+        <v>3552</v>
+      </c>
+      <c r="C20" s="55" t="s">
+        <v>3572</v>
+      </c>
+      <c r="D20" s="53" t="s">
+        <v>3312</v>
+      </c>
+      <c r="E20" s="50">
+        <v>-17.2660801</v>
       </c>
       <c r="F20" s="50">
-        <v>-17.2660801</v>
-      </c>
-      <c r="G20" s="50">
         <v>145.48585990000001</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:6">
       <c r="A21" s="53" t="s">
         <v>1335</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="55" t="s">
-        <v>3571</v>
-      </c>
-      <c r="E21" s="53" t="s">
-        <v>3314</v>
+        <v>3552</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>3570</v>
+      </c>
+      <c r="D21" s="53" t="s">
+        <v>3313</v>
+      </c>
+      <c r="E21" s="50">
+        <v>27.641839000000001</v>
       </c>
       <c r="F21" s="50">
-        <v>27.641839000000001</v>
-      </c>
-      <c r="G21" s="50">
         <v>90.677304599999999</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:6">
       <c r="A22" s="53" t="s">
         <v>1348</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="55" t="s">
-        <v>3574</v>
-      </c>
-      <c r="E22" s="53" t="s">
-        <v>3315</v>
+        <v>3552</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>3573</v>
+      </c>
+      <c r="D22" s="53" t="s">
+        <v>3314</v>
+      </c>
+      <c r="E22" s="50">
+        <v>13.3550091</v>
       </c>
       <c r="F22" s="50">
-        <v>13.3550091</v>
-      </c>
-      <c r="G22" s="50">
         <v>103.85517299999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:6">
       <c r="A23" s="53" t="s">
         <v>1359</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="55" t="s">
-        <v>3575</v>
-      </c>
-      <c r="E23" s="53" t="s">
-        <v>3316</v>
+        <v>3552</v>
+      </c>
+      <c r="C23" s="55" t="s">
+        <v>3574</v>
+      </c>
+      <c r="D23" s="53" t="s">
+        <v>3315</v>
+      </c>
+      <c r="E23" s="50">
+        <v>9.9784936000000002</v>
       </c>
       <c r="F23" s="50">
-        <v>9.9784936000000002</v>
-      </c>
-      <c r="G23" s="50">
         <v>-84.373839399999994</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:6">
       <c r="A24" s="53" t="s">
         <v>1368</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="55" t="s">
-        <v>3576</v>
-      </c>
-      <c r="E24" s="53" t="s">
-        <v>3317</v>
+        <v>3552</v>
+      </c>
+      <c r="C24" s="55" t="s">
+        <v>3575</v>
+      </c>
+      <c r="D24" s="53" t="s">
+        <v>3316</v>
+      </c>
+      <c r="E24" s="50">
+        <v>9.4165520999999899</v>
       </c>
       <c r="F24" s="50">
-        <v>9.4165520999999899</v>
-      </c>
-      <c r="G24" s="50">
         <v>-82.520778699999994</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:6">
       <c r="A25" s="53" t="s">
         <v>1374</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="55" t="s">
-        <v>3570</v>
-      </c>
-      <c r="E25" s="53" t="s">
-        <v>3318</v>
+        <v>3552</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>3569</v>
+      </c>
+      <c r="D25" s="53" t="s">
+        <v>3317</v>
+      </c>
+      <c r="E25" s="50">
+        <v>-13.53195</v>
       </c>
       <c r="F25" s="50">
-        <v>-13.53195</v>
-      </c>
-      <c r="G25" s="50">
         <v>-71.967462599999905</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:6">
       <c r="A26" s="52" t="s">
         <v>1382</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="55" t="s">
-        <v>3577</v>
-      </c>
-      <c r="E26" s="53" t="s">
-        <v>3319</v>
+        <v>3552</v>
+      </c>
+      <c r="C26" s="55" t="s">
+        <v>3576</v>
+      </c>
+      <c r="D26" s="53" t="s">
+        <v>3318</v>
+      </c>
+      <c r="E26" s="50">
+        <v>-3.3175192999999998</v>
       </c>
       <c r="F26" s="50">
-        <v>-3.3175192999999998</v>
-      </c>
-      <c r="G26" s="50">
         <v>35.734195300000003</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:6">
       <c r="A27" s="53" t="s">
         <v>1394</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="55" t="s">
-        <v>3572</v>
-      </c>
-      <c r="E27" s="53" t="s">
-        <v>3320</v>
+        <v>3552</v>
+      </c>
+      <c r="C27" s="55" t="s">
+        <v>3571</v>
+      </c>
+      <c r="D27" s="53" t="s">
+        <v>3319</v>
+      </c>
+      <c r="E27" s="50">
+        <v>21.511236499999999</v>
       </c>
       <c r="F27" s="50">
-        <v>21.511236499999999</v>
-      </c>
-      <c r="G27" s="50">
         <v>-71.518979999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:6">
       <c r="A28" s="52" t="s">
         <v>1399</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="54" t="s">
-        <v>3579</v>
-      </c>
-      <c r="E28" s="53" t="s">
-        <v>3321</v>
+        <v>3552</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>3578</v>
+      </c>
+      <c r="D28" s="53" t="s">
+        <v>3320</v>
+      </c>
+      <c r="E28" s="50">
+        <v>35.689487499999998</v>
       </c>
       <c r="F28" s="50">
-        <v>35.689487499999998</v>
-      </c>
-      <c r="G28" s="50">
         <v>139.69170639999999</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:6">
       <c r="A29" s="52" t="s">
         <v>2818</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="54" t="s">
-        <v>3580</v>
-      </c>
-      <c r="E29" s="53" t="s">
-        <v>3322</v>
+        <v>3552</v>
+      </c>
+      <c r="C29" s="54" t="s">
+        <v>3579</v>
+      </c>
+      <c r="D29" s="53" t="s">
+        <v>3321</v>
+      </c>
+      <c r="E29" s="50">
+        <v>40.416775399999999</v>
       </c>
       <c r="F29" s="50">
-        <v>40.416775399999999</v>
-      </c>
-      <c r="G29" s="50">
         <v>-3.7037901999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:6">
       <c r="A30" s="52" t="s">
         <v>1795</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="54" t="s">
-        <v>3581</v>
-      </c>
-      <c r="E30" s="53" t="s">
-        <v>3323</v>
+        <v>3552</v>
+      </c>
+      <c r="C30" s="54" t="s">
+        <v>3580</v>
+      </c>
+      <c r="D30" s="53" t="s">
+        <v>3322</v>
+      </c>
+      <c r="E30" s="50">
+        <v>39.904199899999902</v>
       </c>
       <c r="F30" s="50">
-        <v>39.904199899999902</v>
-      </c>
-      <c r="G30" s="50">
         <v>116.4073963</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:6">
       <c r="A31" s="52" t="s">
         <v>1841</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="54" t="s">
-        <v>3565</v>
-      </c>
-      <c r="E31" s="53" t="s">
-        <v>3324</v>
+        <v>3552</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>3564</v>
+      </c>
+      <c r="D31" s="53" t="s">
+        <v>3323</v>
+      </c>
+      <c r="E31" s="50">
+        <v>-36.848459699999999</v>
       </c>
       <c r="F31" s="50">
-        <v>-36.848459699999999</v>
-      </c>
-      <c r="G31" s="50">
         <v>174.76333149999999</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:6">
       <c r="A32" s="52" t="s">
         <v>2171</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="54" t="s">
-        <v>3566</v>
-      </c>
-      <c r="E32" s="53" t="s">
-        <v>3325</v>
+        <v>3552</v>
+      </c>
+      <c r="C32" s="54" t="s">
+        <v>3565</v>
+      </c>
+      <c r="D32" s="53" t="s">
+        <v>3324</v>
+      </c>
+      <c r="E32" s="50">
+        <v>55.864237000000003</v>
       </c>
       <c r="F32" s="50">
-        <v>55.864237000000003</v>
-      </c>
-      <c r="G32" s="50">
         <v>-4.2518060000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:6">
       <c r="A33" s="52" t="s">
         <v>2559</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C33" s="50"/>
-      <c r="D33" s="54" t="s">
-        <v>3567</v>
-      </c>
-      <c r="E33" s="53" t="s">
-        <v>3326</v>
+        <v>3552</v>
+      </c>
+      <c r="C33" s="54" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D33" s="53" t="s">
+        <v>3325</v>
+      </c>
+      <c r="E33" s="50">
+        <v>37.1773363</v>
       </c>
       <c r="F33" s="50">
-        <v>37.1773363</v>
-      </c>
-      <c r="G33" s="50">
         <v>-3.5985570999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:6">
       <c r="A34" s="52" t="s">
         <v>2627</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="54" t="s">
-        <v>3568</v>
-      </c>
-      <c r="E34" s="53" t="s">
-        <v>3327</v>
+        <v>3552</v>
+      </c>
+      <c r="C34" s="54" t="s">
+        <v>3567</v>
+      </c>
+      <c r="D34" s="53" t="s">
+        <v>3326</v>
+      </c>
+      <c r="E34" s="50">
+        <v>52.663836699999997</v>
       </c>
       <c r="F34" s="50">
-        <v>52.663836699999997</v>
-      </c>
-      <c r="G34" s="50">
         <v>-8.6267343000000007</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:6">
       <c r="A35" s="53" t="s">
         <v>2690</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>3553</v>
-      </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="54" t="s">
-        <v>3569</v>
-      </c>
-      <c r="E35" s="53" t="s">
-        <v>3328</v>
+        <v>3552</v>
+      </c>
+      <c r="C35" s="54" t="s">
+        <v>3568</v>
+      </c>
+      <c r="D35" s="53" t="s">
+        <v>3327</v>
+      </c>
+      <c r="E35" s="50">
+        <v>38.907192299999998</v>
       </c>
       <c r="F35" s="50">
-        <v>38.907192299999998</v>
-      </c>
-      <c r="G35" s="50">
         <v>-77.036870699999994</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:A36" xr:uid="{E0F9AFD1-752F-46CC-9D8C-A798927D6393}"/>
-  <sortState ref="A2:G35">
+  <sortState ref="A2:F35">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -54135,10 +54094,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.25">
       <c r="A1" s="43" t="s">
+        <v>3328</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>3329</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>3330</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25">
@@ -54146,164 +54105,164 @@
         <v>25</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>3331</v>
+        <v>3330</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="40" t="s">
+        <v>3331</v>
+      </c>
+      <c r="B3" s="40" t="s">
         <v>3332</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>3333</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="40" t="s">
+        <v>3333</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>3334</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>3335</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25">
       <c r="A5" s="40" t="s">
+        <v>3335</v>
+      </c>
+      <c r="B5" s="40" t="s">
         <v>3336</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>3337</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25">
       <c r="A6" s="40" t="s">
+        <v>3337</v>
+      </c>
+      <c r="B6" s="40" t="s">
         <v>3338</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>3339</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25">
       <c r="A7" s="40" t="s">
+        <v>3339</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>3340</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>3341</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.25">
       <c r="A8" s="40" t="s">
+        <v>3341</v>
+      </c>
+      <c r="B8" s="40" t="s">
         <v>3342</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>3343</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.25">
       <c r="A9" s="40" t="s">
+        <v>3343</v>
+      </c>
+      <c r="B9" s="40" t="s">
         <v>3344</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>3345</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.25">
       <c r="A10" s="40" t="s">
+        <v>3345</v>
+      </c>
+      <c r="B10" s="40" t="s">
         <v>3346</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>3347</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.25">
       <c r="A11" s="40" t="s">
+        <v>3347</v>
+      </c>
+      <c r="B11" s="40" t="s">
         <v>3348</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>3349</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.25">
       <c r="A12" s="40" t="s">
+        <v>3349</v>
+      </c>
+      <c r="B12" s="40" t="s">
         <v>3350</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>3351</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.25">
       <c r="A13" s="40" t="s">
+        <v>3351</v>
+      </c>
+      <c r="B13" s="40" t="s">
         <v>3352</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>3353</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14.25">
       <c r="A14" s="40" t="s">
+        <v>3353</v>
+      </c>
+      <c r="B14" s="40" t="s">
         <v>3354</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>3355</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.25">
       <c r="A15" s="44" t="s">
+        <v>3355</v>
+      </c>
+      <c r="B15" s="44" t="s">
         <v>3356</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>3357</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="14.25">
       <c r="A16" s="40" t="s">
+        <v>3357</v>
+      </c>
+      <c r="B16" s="40" t="s">
         <v>3358</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>3359</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25">
       <c r="A17" s="40" t="s">
+        <v>3359</v>
+      </c>
+      <c r="B17" s="40" t="s">
         <v>3360</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>3361</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25">
       <c r="A18" s="40" t="s">
+        <v>3361</v>
+      </c>
+      <c r="B18" s="40" t="s">
         <v>3362</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>3363</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25">
       <c r="A19" s="40" t="s">
+        <v>3363</v>
+      </c>
+      <c r="B19" s="40" t="s">
         <v>3364</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>3365</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25">
       <c r="A20" s="44" t="s">
+        <v>3365</v>
+      </c>
+      <c r="B20" s="44" t="s">
         <v>3366</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>3367</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25">
       <c r="A21" s="44" t="s">
+        <v>3367</v>
+      </c>
+      <c r="B21" s="44" t="s">
         <v>3368</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>3369</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25">
       <c r="A22" s="40" t="s">
-        <v>3370</v>
+        <v>3369</v>
       </c>
       <c r="B22" s="40" t="s">
         <v>1560</v>
@@ -54311,31 +54270,31 @@
     </row>
     <row r="23" spans="1:2" ht="14.25">
       <c r="A23" s="40" t="s">
+        <v>3370</v>
+      </c>
+      <c r="B23" s="40" t="s">
         <v>3371</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>3372</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25">
       <c r="A24" s="40" t="s">
+        <v>3372</v>
+      </c>
+      <c r="B24" s="40" t="s">
         <v>3373</v>
-      </c>
-      <c r="B24" s="40" t="s">
-        <v>3374</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25">
       <c r="A25" s="40" t="s">
+        <v>3374</v>
+      </c>
+      <c r="B25" s="40" t="s">
         <v>3375</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>3376</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25">
       <c r="A26" s="40" t="s">
-        <v>3377</v>
+        <v>3376</v>
       </c>
       <c r="B26" s="40" t="s">
         <v>118</v>
@@ -54343,23 +54302,23 @@
     </row>
     <row r="27" spans="1:2" ht="14.25">
       <c r="A27" s="44" t="s">
+        <v>3377</v>
+      </c>
+      <c r="B27" s="44" t="s">
         <v>3378</v>
-      </c>
-      <c r="B27" s="44" t="s">
-        <v>3379</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25">
       <c r="A28" s="40" t="s">
+        <v>3379</v>
+      </c>
+      <c r="B28" s="40" t="s">
         <v>3380</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>3381</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25">
       <c r="A29" s="40" t="s">
-        <v>3382</v>
+        <v>3381</v>
       </c>
       <c r="B29" s="40" t="s">
         <v>978</v>
@@ -54367,31 +54326,31 @@
     </row>
     <row r="30" spans="1:2" ht="14.25">
       <c r="A30" s="40" t="s">
+        <v>3382</v>
+      </c>
+      <c r="B30" s="40" t="s">
         <v>3383</v>
-      </c>
-      <c r="B30" s="40" t="s">
-        <v>3384</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25">
       <c r="A31" s="40" t="s">
+        <v>3384</v>
+      </c>
+      <c r="B31" s="40" t="s">
         <v>3385</v>
-      </c>
-      <c r="B31" s="40" t="s">
-        <v>3386</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25">
       <c r="A32" s="40" t="s">
+        <v>3386</v>
+      </c>
+      <c r="B32" s="40" t="s">
         <v>3387</v>
-      </c>
-      <c r="B32" s="40" t="s">
-        <v>3388</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25">
       <c r="A33" s="40" t="s">
-        <v>3389</v>
+        <v>3388</v>
       </c>
       <c r="B33" s="40" t="s">
         <v>83</v>
@@ -54399,15 +54358,15 @@
     </row>
     <row r="34" spans="1:2" ht="14.25">
       <c r="A34" s="40" t="s">
+        <v>3389</v>
+      </c>
+      <c r="B34" s="40" t="s">
         <v>3390</v>
-      </c>
-      <c r="B34" s="40" t="s">
-        <v>3391</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25">
       <c r="A35" s="40" t="s">
-        <v>3392</v>
+        <v>3391</v>
       </c>
       <c r="B35" s="40" t="s">
         <v>2197</v>
@@ -54415,15 +54374,15 @@
     </row>
     <row r="36" spans="1:2" ht="14.25">
       <c r="A36" s="40" t="s">
+        <v>3392</v>
+      </c>
+      <c r="B36" s="40" t="s">
         <v>3393</v>
-      </c>
-      <c r="B36" s="40" t="s">
-        <v>3394</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25">
       <c r="A37" s="40" t="s">
-        <v>3395</v>
+        <v>3394</v>
       </c>
       <c r="B37" s="40" t="s">
         <v>1507</v>
@@ -54431,87 +54390,87 @@
     </row>
     <row r="38" spans="1:2" ht="14.25">
       <c r="A38" s="40" t="s">
+        <v>3395</v>
+      </c>
+      <c r="B38" s="40" t="s">
         <v>3396</v>
-      </c>
-      <c r="B38" s="40" t="s">
-        <v>3397</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25">
       <c r="A39" s="40" t="s">
+        <v>3397</v>
+      </c>
+      <c r="B39" s="40" t="s">
         <v>3398</v>
-      </c>
-      <c r="B39" s="40" t="s">
-        <v>3399</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25">
       <c r="A40" s="40" t="s">
+        <v>3399</v>
+      </c>
+      <c r="B40" s="40" t="s">
         <v>3400</v>
-      </c>
-      <c r="B40" s="40" t="s">
-        <v>3401</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25">
       <c r="A41" s="40" t="s">
+        <v>3401</v>
+      </c>
+      <c r="B41" s="40" t="s">
         <v>3402</v>
-      </c>
-      <c r="B41" s="40" t="s">
-        <v>3403</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25">
       <c r="A42" s="40" t="s">
+        <v>3403</v>
+      </c>
+      <c r="B42" s="40" t="s">
         <v>3404</v>
-      </c>
-      <c r="B42" s="40" t="s">
-        <v>3405</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25">
       <c r="A43" s="44" t="s">
+        <v>3405</v>
+      </c>
+      <c r="B43" s="44" t="s">
         <v>3406</v>
-      </c>
-      <c r="B43" s="44" t="s">
-        <v>3407</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25">
       <c r="A44" s="44" t="s">
+        <v>3407</v>
+      </c>
+      <c r="B44" s="44" t="s">
         <v>3408</v>
-      </c>
-      <c r="B44" s="44" t="s">
-        <v>3409</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25">
       <c r="A45" s="44" t="s">
+        <v>3409</v>
+      </c>
+      <c r="B45" s="44" t="s">
         <v>3410</v>
-      </c>
-      <c r="B45" s="44" t="s">
-        <v>3411</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25">
       <c r="A46" s="44" t="s">
+        <v>3411</v>
+      </c>
+      <c r="B46" s="44" t="s">
         <v>3412</v>
-      </c>
-      <c r="B46" s="44" t="s">
-        <v>3413</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25">
       <c r="A47" s="41" t="s">
+        <v>3413</v>
+      </c>
+      <c r="B47" s="41" t="s">
         <v>3414</v>
-      </c>
-      <c r="B47" s="41" t="s">
-        <v>3415</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25">
       <c r="A48" s="41" t="s">
-        <v>3416</v>
+        <v>3415</v>
       </c>
       <c r="B48" s="41" t="s">
         <v>990</v>
@@ -54519,95 +54478,95 @@
     </row>
     <row r="49" spans="1:2" ht="14.25">
       <c r="A49" s="44" t="s">
+        <v>3416</v>
+      </c>
+      <c r="B49" s="44" t="s">
         <v>3417</v>
-      </c>
-      <c r="B49" s="44" t="s">
-        <v>3418</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25">
       <c r="A50" s="44" t="s">
+        <v>3418</v>
+      </c>
+      <c r="B50" s="44" t="s">
         <v>3419</v>
-      </c>
-      <c r="B50" s="44" t="s">
-        <v>3420</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25">
       <c r="A51" s="44" t="s">
+        <v>3420</v>
+      </c>
+      <c r="B51" s="44" t="s">
         <v>3421</v>
-      </c>
-      <c r="B51" s="44" t="s">
-        <v>3422</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25">
       <c r="A52" s="41" t="s">
+        <v>3422</v>
+      </c>
+      <c r="B52" s="41" t="s">
         <v>3423</v>
-      </c>
-      <c r="B52" s="41" t="s">
-        <v>3424</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25">
       <c r="A53" s="41" t="s">
+        <v>3424</v>
+      </c>
+      <c r="B53" s="41" t="s">
         <v>3425</v>
-      </c>
-      <c r="B53" s="41" t="s">
-        <v>3426</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25">
       <c r="A54" s="41" t="s">
+        <v>3426</v>
+      </c>
+      <c r="B54" s="41" t="s">
         <v>3427</v>
-      </c>
-      <c r="B54" s="41" t="s">
-        <v>3428</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25">
       <c r="A55" s="41" t="s">
+        <v>3428</v>
+      </c>
+      <c r="B55" s="41" t="s">
         <v>3429</v>
-      </c>
-      <c r="B55" s="41" t="s">
-        <v>3430</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25">
       <c r="A56" s="41" t="s">
+        <v>3430</v>
+      </c>
+      <c r="B56" s="41" t="s">
         <v>3431</v>
-      </c>
-      <c r="B56" s="41" t="s">
-        <v>3432</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25">
       <c r="A57" s="41" t="s">
+        <v>3432</v>
+      </c>
+      <c r="B57" s="41" t="s">
         <v>3433</v>
-      </c>
-      <c r="B57" s="41" t="s">
-        <v>3434</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25">
       <c r="A58" s="44" t="s">
+        <v>3434</v>
+      </c>
+      <c r="B58" s="44" t="s">
         <v>3435</v>
-      </c>
-      <c r="B58" s="44" t="s">
-        <v>3436</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.25">
       <c r="A59" s="41" t="s">
+        <v>3436</v>
+      </c>
+      <c r="B59" s="41" t="s">
         <v>3437</v>
-      </c>
-      <c r="B59" s="41" t="s">
-        <v>3438</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25">
       <c r="A60" s="41" t="s">
-        <v>3439</v>
+        <v>3438</v>
       </c>
       <c r="B60" s="41" t="s">
         <v>844</v>
@@ -54615,15 +54574,15 @@
     </row>
     <row r="61" spans="1:2" ht="14.25">
       <c r="A61" s="41" t="s">
+        <v>3439</v>
+      </c>
+      <c r="B61" s="41" t="s">
         <v>3440</v>
-      </c>
-      <c r="B61" s="41" t="s">
-        <v>3441</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="14.25">
       <c r="A62" s="41" t="s">
-        <v>3442</v>
+        <v>3441</v>
       </c>
       <c r="B62" s="41" t="s">
         <v>888</v>
@@ -54631,23 +54590,23 @@
     </row>
     <row r="63" spans="1:2" ht="14.25">
       <c r="A63" s="41" t="s">
+        <v>3442</v>
+      </c>
+      <c r="B63" s="41" t="s">
         <v>3443</v>
-      </c>
-      <c r="B63" s="41" t="s">
-        <v>3444</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="14.25">
       <c r="A64" s="41" t="s">
+        <v>3444</v>
+      </c>
+      <c r="B64" s="41" t="s">
         <v>3445</v>
-      </c>
-      <c r="B64" s="41" t="s">
-        <v>3446</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="14.25">
       <c r="A65" s="41" t="s">
-        <v>3447</v>
+        <v>3446</v>
       </c>
       <c r="B65" s="41" t="s">
         <v>2850</v>
@@ -54655,39 +54614,39 @@
     </row>
     <row r="66" spans="1:2" ht="14.25">
       <c r="A66" s="44" t="s">
+        <v>3447</v>
+      </c>
+      <c r="B66" s="44" t="s">
         <v>3448</v>
-      </c>
-      <c r="B66" s="44" t="s">
-        <v>3449</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="14.25">
       <c r="A67" s="41" t="s">
+        <v>3449</v>
+      </c>
+      <c r="B67" s="41" t="s">
         <v>3450</v>
-      </c>
-      <c r="B67" s="41" t="s">
-        <v>3451</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="14.25">
       <c r="A68" s="41" t="s">
+        <v>3451</v>
+      </c>
+      <c r="B68" s="41" t="s">
         <v>3452</v>
-      </c>
-      <c r="B68" s="41" t="s">
-        <v>3453</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="14.25">
       <c r="A69" s="41" t="s">
+        <v>3453</v>
+      </c>
+      <c r="B69" s="41" t="s">
         <v>3454</v>
-      </c>
-      <c r="B69" s="41" t="s">
-        <v>3455</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="14.25">
       <c r="A70" s="41" t="s">
-        <v>3456</v>
+        <v>3455</v>
       </c>
       <c r="B70" s="41" t="s">
         <v>359</v>
@@ -54695,74 +54654,74 @@
     </row>
     <row r="71" spans="1:2" ht="14.25">
       <c r="A71" s="41" t="s">
+        <v>3456</v>
+      </c>
+      <c r="B71" s="41" t="s">
         <v>3457</v>
-      </c>
-      <c r="B71" s="41" t="s">
-        <v>3458</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="14.25">
       <c r="A72" s="41" t="s">
+        <v>3458</v>
+      </c>
+      <c r="B72" s="41" t="s">
         <v>3459</v>
-      </c>
-      <c r="B72" s="41" t="s">
-        <v>3460</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="14.25">
       <c r="A73" s="41" t="s">
+        <v>3460</v>
+      </c>
+      <c r="B73" s="41" t="s">
         <v>3461</v>
-      </c>
-      <c r="B73" s="41" t="s">
-        <v>3462</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="14.25">
       <c r="A74" s="44" t="s">
+        <v>3462</v>
+      </c>
+      <c r="B74" s="44" t="s">
         <v>3463</v>
-      </c>
-      <c r="B74" s="44" t="s">
-        <v>3464</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="14.25">
       <c r="A75" s="44" t="s">
+        <v>3464</v>
+      </c>
+      <c r="B75" s="44" t="s">
         <v>3465</v>
-      </c>
-      <c r="B75" s="44" t="s">
-        <v>3466</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="14.25">
       <c r="A76" s="41" t="s">
+        <v>3466</v>
+      </c>
+      <c r="B76" s="41" t="s">
         <v>3467</v>
-      </c>
-      <c r="B76" s="41" t="s">
-        <v>3468</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.25">
       <c r="A77" s="41" t="s">
+        <v>3468</v>
+      </c>
+      <c r="B77" s="41" t="s">
         <v>3469</v>
-      </c>
-      <c r="B77" s="41" t="s">
-        <v>3470</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="14.25">
       <c r="A78" s="44" t="s">
+        <v>3470</v>
+      </c>
+      <c r="B78" s="44" t="s">
         <v>3471</v>
-      </c>
-      <c r="B78" s="44" t="s">
-        <v>3472</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="14.25">
       <c r="A79" s="41" t="s">
+        <v>3472</v>
+      </c>
+      <c r="B79" s="41" t="s">
         <v>3473</v>
-      </c>
-      <c r="B79" s="41" t="s">
-        <v>3474</v>
       </c>
     </row>
   </sheetData>
@@ -54786,555 +54745,555 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14.25">
       <c r="A1" s="45" t="s">
+        <v>3474</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>3337</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>3475</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>3338</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>3476</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25">
       <c r="A2" s="42" t="s">
+        <v>3476</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>3477</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="C2" s="42" t="s">
         <v>3478</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>3479</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25">
       <c r="A3" s="45" t="s">
-        <v>3480</v>
+        <v>3479</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>3342</v>
+        <v>3341</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25">
       <c r="A4" s="45" t="s">
-        <v>3481</v>
+        <v>3480</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>3340</v>
+        <v>3339</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25">
       <c r="A5" s="45" t="s">
+        <v>3481</v>
+      </c>
+      <c r="B5" s="45" t="s">
         <v>3482</v>
       </c>
-      <c r="B5" s="45" t="s">
-        <v>3483</v>
-      </c>
       <c r="C5" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25">
       <c r="A6" s="45" t="s">
+        <v>3483</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>3349</v>
+      </c>
+      <c r="C6" s="42" t="s">
         <v>3484</v>
-      </c>
-      <c r="B6" s="45" t="s">
-        <v>3350</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>3485</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25">
       <c r="A7" s="45" t="s">
-        <v>3486</v>
+        <v>3485</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>3352</v>
+        <v>3351</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25">
       <c r="A8" s="45" t="s">
+        <v>3486</v>
+      </c>
+      <c r="B8" s="45" t="s">
         <v>3487</v>
       </c>
-      <c r="B8" s="45" t="s">
-        <v>3488</v>
-      </c>
       <c r="C8" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25">
       <c r="A9" s="45" t="s">
+        <v>3488</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>3355</v>
+      </c>
+      <c r="C9" s="42" t="s">
         <v>3489</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>3356</v>
-      </c>
-      <c r="C9" s="42" t="s">
-        <v>3490</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25">
       <c r="A10" s="45" t="s">
+        <v>3490</v>
+      </c>
+      <c r="B10" s="45" t="s">
         <v>3491</v>
       </c>
-      <c r="B10" s="45" t="s">
-        <v>3492</v>
-      </c>
       <c r="C10" s="42" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25">
       <c r="A11" s="45" t="s">
-        <v>3493</v>
+        <v>3492</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>3360</v>
+        <v>3359</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25">
       <c r="A12" s="45" t="s">
+        <v>3493</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>3361</v>
+      </c>
+      <c r="C12" s="42" t="s">
         <v>3494</v>
-      </c>
-      <c r="B12" s="45" t="s">
-        <v>3362</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>3495</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25">
       <c r="A13" s="45" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>3368</v>
+        <v>3367</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25">
       <c r="A14" s="45" t="s">
-        <v>3496</v>
+        <v>3495</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>3370</v>
+        <v>3369</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25">
       <c r="A15" s="45" t="s">
-        <v>3497</v>
+        <v>3496</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>3371</v>
+        <v>3370</v>
       </c>
       <c r="C15" s="42"/>
     </row>
     <row r="16" spans="1:3" ht="14.25">
       <c r="A16" s="45" t="s">
-        <v>3498</v>
+        <v>3497</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>3373</v>
+        <v>3372</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25">
       <c r="A17" s="45" t="s">
-        <v>3499</v>
+        <v>3498</v>
       </c>
       <c r="B17" s="45" t="s">
         <v>1124</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25">
       <c r="A18" s="45" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
       <c r="B18" s="45" t="s">
-        <v>3377</v>
+        <v>3376</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25">
       <c r="A19" s="45" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>3378</v>
+        <v>3377</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25">
       <c r="A20" s="45" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>3380</v>
+        <v>3379</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25">
       <c r="A21" s="45" t="s">
-        <v>3503</v>
+        <v>3502</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>3389</v>
+        <v>3388</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25">
       <c r="A22" s="45" t="s">
-        <v>3504</v>
+        <v>3503</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>3390</v>
+        <v>3389</v>
       </c>
       <c r="C22" s="42"/>
     </row>
     <row r="23" spans="1:3" ht="14.25">
       <c r="A23" s="45" t="s">
+        <v>3504</v>
+      </c>
+      <c r="B23" s="45" t="s">
         <v>3505</v>
       </c>
-      <c r="B23" s="45" t="s">
+      <c r="C23" s="42" t="s">
         <v>3506</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>3507</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25">
       <c r="A24" s="45" t="s">
-        <v>3508</v>
+        <v>3507</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>3393</v>
+        <v>3392</v>
       </c>
       <c r="C24" s="42"/>
     </row>
     <row r="25" spans="1:3" ht="14.25">
       <c r="A25" s="45" t="s">
-        <v>3509</v>
+        <v>3508</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>3395</v>
+        <v>3394</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25">
       <c r="A26" s="45" t="s">
-        <v>3510</v>
+        <v>3509</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>3396</v>
+        <v>3395</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25">
       <c r="A27" s="45" t="s">
-        <v>3406</v>
+        <v>3405</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>3406</v>
+        <v>3405</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>3406</v>
+        <v>3405</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25">
       <c r="A28" s="45" t="s">
-        <v>3511</v>
+        <v>3510</v>
       </c>
       <c r="B28" s="45" t="s">
-        <v>3408</v>
+        <v>3407</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25">
       <c r="A29" s="45" t="s">
+        <v>3511</v>
+      </c>
+      <c r="B29" s="45" t="s">
         <v>3512</v>
       </c>
-      <c r="B29" s="45" t="s">
-        <v>3513</v>
-      </c>
       <c r="C29" s="42" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25">
       <c r="A30" s="45" t="s">
-        <v>3514</v>
+        <v>3513</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>3423</v>
+        <v>3422</v>
       </c>
       <c r="C30" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25">
       <c r="A31" s="45" t="s">
-        <v>3515</v>
+        <v>3514</v>
       </c>
       <c r="B31" s="45" t="s">
-        <v>3425</v>
+        <v>3424</v>
       </c>
       <c r="C31" s="42" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25">
       <c r="A32" s="45" t="s">
-        <v>3516</v>
+        <v>3515</v>
       </c>
       <c r="B32" s="45" t="s">
-        <v>3427</v>
+        <v>3426</v>
       </c>
       <c r="C32" s="42"/>
     </row>
     <row r="33" spans="1:3" ht="14.25">
       <c r="A33" s="45" t="s">
+        <v>3516</v>
+      </c>
+      <c r="B33" s="45" t="s">
         <v>3517</v>
       </c>
-      <c r="B33" s="45" t="s">
-        <v>3518</v>
-      </c>
       <c r="C33" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25">
       <c r="A34" s="45" t="s">
-        <v>3519</v>
+        <v>3518</v>
       </c>
       <c r="B34" s="45" t="s">
-        <v>3431</v>
+        <v>3430</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25">
       <c r="A35" s="45" t="s">
-        <v>3520</v>
+        <v>3519</v>
       </c>
       <c r="B35" s="45" t="s">
-        <v>3433</v>
+        <v>3432</v>
       </c>
       <c r="C35" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25">
       <c r="A36" s="45" t="s">
-        <v>3521</v>
+        <v>3520</v>
       </c>
       <c r="B36" s="45" t="s">
-        <v>3435</v>
+        <v>3434</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>3507</v>
+        <v>3506</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25">
       <c r="A37" s="45" t="s">
-        <v>3522</v>
+        <v>3521</v>
       </c>
       <c r="B37" s="45" t="s">
-        <v>3437</v>
+        <v>3436</v>
       </c>
       <c r="C37" s="42" t="s">
-        <v>3507</v>
+        <v>3506</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25">
       <c r="A38" s="45" t="s">
-        <v>3523</v>
+        <v>3522</v>
       </c>
       <c r="B38" s="45" t="s">
-        <v>3440</v>
+        <v>3439</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25">
       <c r="A39" s="45" t="s">
-        <v>3524</v>
+        <v>3523</v>
       </c>
       <c r="B39" s="45" t="s">
-        <v>3442</v>
+        <v>3441</v>
       </c>
       <c r="C39" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25">
       <c r="A40" s="45" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="B40" s="45" t="s">
-        <v>3443</v>
+        <v>3442</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>3495</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25">
       <c r="A41" s="45" t="s">
-        <v>3526</v>
+        <v>3525</v>
       </c>
       <c r="B41" s="45" t="s">
-        <v>3445</v>
+        <v>3444</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25">
       <c r="A42" s="45" t="s">
-        <v>3527</v>
+        <v>3526</v>
       </c>
       <c r="B42" s="45" t="s">
-        <v>3447</v>
+        <v>3446</v>
       </c>
       <c r="C42" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25">
       <c r="A43" s="45" t="s">
-        <v>3528</v>
+        <v>3527</v>
       </c>
       <c r="B43" s="45" t="s">
-        <v>3450</v>
+        <v>3449</v>
       </c>
       <c r="C43" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25">
       <c r="A44" s="45" t="s">
-        <v>3529</v>
+        <v>3528</v>
       </c>
       <c r="B44" s="45" t="s">
-        <v>3454</v>
+        <v>3453</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25">
       <c r="A45" s="45" t="s">
-        <v>3530</v>
+        <v>3529</v>
       </c>
       <c r="B45" s="45" t="s">
-        <v>3461</v>
+        <v>3460</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>3495</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25">
       <c r="A46" s="45" t="s">
-        <v>3531</v>
+        <v>3530</v>
       </c>
       <c r="B46" s="45" t="s">
-        <v>3457</v>
+        <v>3456</v>
       </c>
       <c r="C46" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25">
       <c r="A47" s="45" t="s">
+        <v>3531</v>
+      </c>
+      <c r="B47" s="45" t="s">
         <v>3532</v>
       </c>
-      <c r="B47" s="45" t="s">
-        <v>3533</v>
-      </c>
       <c r="C47" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25">
       <c r="A48" s="45" t="s">
-        <v>3534</v>
+        <v>3533</v>
       </c>
       <c r="B48" s="45" t="s">
-        <v>3463</v>
+        <v>3462</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>3495</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25">
       <c r="A49" s="45" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="B49" s="45" t="s">
-        <v>3467</v>
+        <v>3466</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25">
       <c r="A50" s="45" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
       <c r="B50" s="45" t="s">
-        <v>3473</v>
+        <v>3472</v>
       </c>
       <c r="C50" s="42" t="s">
-        <v>3476</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25">
       <c r="A51" s="45" t="s">
-        <v>3537</v>
+        <v>3536</v>
       </c>
       <c r="B51" s="45" t="s">
-        <v>3469</v>
+        <v>3468</v>
       </c>
       <c r="C51" s="42" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
     </row>
   </sheetData>
@@ -55357,12 +55316,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="13.9">
       <c r="A1" s="46" t="s">
-        <v>3538</v>
+        <v>3537</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="13.9">
       <c r="A2" s="46" t="s">
-        <v>3539</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.9">
@@ -55382,17 +55341,17 @@
     </row>
     <row r="6" spans="1:1" ht="13.9">
       <c r="A6" s="46" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="13.9">
       <c r="A7" s="46" t="s">
-        <v>3424</v>
+        <v>3423</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="13.9">
       <c r="A8" s="46" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="13.9">
@@ -55407,12 +55366,12 @@
     </row>
     <row r="11" spans="1:1" ht="13.9">
       <c r="A11" s="46" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="13.9">
       <c r="A12" s="46" t="s">
-        <v>3543</v>
+        <v>3542</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="13.9">
@@ -55422,17 +55381,17 @@
     </row>
     <row r="14" spans="1:1" ht="13.9">
       <c r="A14" s="46" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="13.9">
       <c r="A15" s="46" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="13.9">
       <c r="A16" s="46" t="s">
-        <v>3546</v>
+        <v>3545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>